<commit_message>
added new crime marker icons
</commit_message>
<xml_diff>
--- a/data/crime_data_with_lat_long.xlsx
+++ b/data/crime_data_with_lat_long.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\jalen\Classes\CAPSTONE\crimeData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/allysonvasquez/Developer/4155_StreetSafe/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{20DEE670-075C-46AB-9BC1-551E58363600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5007D783-8885-AA42-A80F-BAA3F82EC626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="26640" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1 - crime_data" sheetId="1" r:id="rId1"/>
@@ -1330,7 +1330,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -2742,22 +2742,22 @@
   <dimension ref="A1:G151"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:J2"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.28515625" defaultRowHeight="20.100000000000001" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="34.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="12" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.28515625" style="1"/>
+    <col min="8" max="16384" width="8.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20.25" customHeight="1">
+    <row r="1" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2780,7 +2780,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="20.25" customHeight="1">
+    <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -2803,7 +2803,7 @@
         <v>35.305999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="3" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>9</v>
       </c>
@@ -2826,7 +2826,7 @@
         <v>35.324750000000002</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="4" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
         <v>12</v>
       </c>
@@ -2849,7 +2849,7 @@
         <v>35.31561</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="5" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
         <v>15</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>35.291730000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="6" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
         <v>18</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>35.321579999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="7" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
         <v>21</v>
       </c>
@@ -2918,7 +2918,7 @@
         <v>35.297159999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="8" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
         <v>24</v>
       </c>
@@ -2941,7 +2941,7 @@
         <v>35.293379999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="9" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
         <v>12</v>
       </c>
@@ -2964,7 +2964,7 @@
         <v>35.300980000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="10" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
         <v>29</v>
       </c>
@@ -2987,7 +2987,7 @@
         <v>35.316290000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="11" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="6" t="s">
         <v>32</v>
       </c>
@@ -3010,7 +3010,7 @@
         <v>35.304119999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="12" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="6" t="s">
         <v>35</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>35.292389999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="13" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="6" t="s">
         <v>38</v>
       </c>
@@ -3056,7 +3056,7 @@
         <v>35.296219999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="14" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="6" t="s">
         <v>21</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>35.291260000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="15" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="6" t="s">
         <v>32</v>
       </c>
@@ -3102,7 +3102,7 @@
         <v>35.30827</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="16" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="6" t="s">
         <v>12</v>
       </c>
@@ -3125,7 +3125,7 @@
         <v>35.328400000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="17" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="6" t="s">
         <v>47</v>
       </c>
@@ -3148,7 +3148,7 @@
         <v>35.300980000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="18" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="6" t="s">
         <v>50</v>
       </c>
@@ -3171,7 +3171,7 @@
         <v>35.30827</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="19" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="6" t="s">
         <v>35</v>
       </c>
@@ -3194,7 +3194,7 @@
         <v>35.306789999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="20" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="6" t="s">
         <v>24</v>
       </c>
@@ -3217,7 +3217,7 @@
         <v>35.296219999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="21" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="6" t="s">
         <v>9</v>
       </c>
@@ -3240,7 +3240,7 @@
         <v>35.308540000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="22" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="6" t="s">
         <v>32</v>
       </c>
@@ -3263,7 +3263,7 @@
         <v>35.297800000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="23" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="6" t="s">
         <v>12</v>
       </c>
@@ -3286,7 +3286,7 @@
         <v>35.30106</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="24" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="6" t="s">
         <v>5</v>
       </c>
@@ -3309,7 +3309,7 @@
         <v>35.316949999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="25" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="6" t="s">
         <v>32</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>35.283859999999997</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="26" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="6" t="s">
         <v>18</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>35.314360000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="27" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="6" t="s">
         <v>50</v>
       </c>
@@ -3378,7 +3378,7 @@
         <v>35.305759999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="28" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="6" t="s">
         <v>32</v>
       </c>
@@ -3401,7 +3401,7 @@
         <v>35.327869999999997</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="29" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="6" t="s">
         <v>73</v>
       </c>
@@ -3424,7 +3424,7 @@
         <v>35.306789999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="30" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="6" t="s">
         <v>9</v>
       </c>
@@ -3447,7 +3447,7 @@
         <v>35.308709999999998</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="31" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="6" t="s">
         <v>21</v>
       </c>
@@ -3470,7 +3470,7 @@
         <v>35.328009999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="32" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="6" t="s">
         <v>32</v>
       </c>
@@ -3493,7 +3493,7 @@
         <v>35.075319999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="33" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="6" t="s">
         <v>32</v>
       </c>
@@ -3516,7 +3516,7 @@
         <v>35.075319999999998</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="34" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="6" t="s">
         <v>32</v>
       </c>
@@ -3539,7 +3539,7 @@
         <v>35.312640000000002</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="35" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="6" t="s">
         <v>21</v>
       </c>
@@ -3562,7 +3562,7 @@
         <v>35.304049999999997</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="36" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="6" t="s">
         <v>32</v>
       </c>
@@ -3585,7 +3585,7 @@
         <v>35.325899999999997</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="37" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="6" t="s">
         <v>5</v>
       </c>
@@ -3608,7 +3608,7 @@
         <v>35.312899999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="38" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="6" t="s">
         <v>38</v>
       </c>
@@ -3631,7 +3631,7 @@
         <v>35.296219999999998</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="39" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="6" t="s">
         <v>38</v>
       </c>
@@ -3654,7 +3654,7 @@
         <v>35.296219999999998</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="40" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="6" t="s">
         <v>21</v>
       </c>
@@ -3677,7 +3677,7 @@
         <v>35.312640000000002</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="41" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="6" t="s">
         <v>5</v>
       </c>
@@ -3700,7 +3700,7 @@
         <v>35.296219999999998</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="42" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="6" t="s">
         <v>100</v>
       </c>
@@ -3723,7 +3723,7 @@
         <v>35.304430000000004</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="43" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="6" t="s">
         <v>50</v>
       </c>
@@ -3746,7 +3746,7 @@
         <v>35.301839999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="44" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="6" t="s">
         <v>15</v>
       </c>
@@ -3769,7 +3769,7 @@
         <v>35.321570000000001</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="45" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="6" t="s">
         <v>9</v>
       </c>
@@ -3792,7 +3792,7 @@
         <v>35.325899999999997</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="46" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="6" t="s">
         <v>47</v>
       </c>
@@ -3815,7 +3815,7 @@
         <v>35.332509999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="47" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="6" t="s">
         <v>9</v>
       </c>
@@ -3838,7 +3838,7 @@
         <v>35.308720000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="48" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="6" t="s">
         <v>5</v>
       </c>
@@ -3861,7 +3861,7 @@
         <v>35.285110000000003</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="49" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="6" t="s">
         <v>32</v>
       </c>
@@ -3884,7 +3884,7 @@
         <v>35.293190000000003</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="50" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="6" t="s">
         <v>47</v>
       </c>
@@ -3907,7 +3907,7 @@
         <v>35.299759999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="51" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="6" t="s">
         <v>32</v>
       </c>
@@ -3930,7 +3930,7 @@
         <v>35.328850000000003</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="52" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="6" t="s">
         <v>5</v>
       </c>
@@ -3953,7 +3953,7 @@
         <v>35.286740000000002</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="53" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="6" t="s">
         <v>32</v>
       </c>
@@ -3976,7 +3976,7 @@
         <v>35.329900000000002</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="54" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="6" t="s">
         <v>21</v>
       </c>
@@ -3999,7 +3999,7 @@
         <v>35.293610000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="55" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="6" t="s">
         <v>21</v>
       </c>
@@ -4022,7 +4022,7 @@
         <v>35.314239999999998</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="56" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="6" t="s">
         <v>129</v>
       </c>
@@ -4045,7 +4045,7 @@
         <v>35.305759999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="57" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="6" t="s">
         <v>21</v>
       </c>
@@ -4068,7 +4068,7 @@
         <v>35.309869999999997</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="58" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="6" t="s">
         <v>5</v>
       </c>
@@ -4091,7 +4091,7 @@
         <v>35.287430000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="59" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="6" t="s">
         <v>21</v>
       </c>
@@ -4114,7 +4114,7 @@
         <v>35.317450000000001</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="60" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="6" t="s">
         <v>32</v>
       </c>
@@ -4137,7 +4137,7 @@
         <v>35.308869999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="61" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="6" t="s">
         <v>15</v>
       </c>
@@ -4160,7 +4160,7 @@
         <v>35.314660000000003</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="62" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="6" t="s">
         <v>32</v>
       </c>
@@ -4183,7 +4183,7 @@
         <v>35.310029999999998</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="63" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="6" t="s">
         <v>50</v>
       </c>
@@ -4206,7 +4206,7 @@
         <v>35.314140000000002</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="64" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="6" t="s">
         <v>32</v>
       </c>
@@ -4229,7 +4229,7 @@
         <v>35.288629999999998</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="65" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="6" t="s">
         <v>148</v>
       </c>
@@ -4252,7 +4252,7 @@
         <v>35.300980000000003</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="66" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="6" t="s">
         <v>21</v>
       </c>
@@ -4275,7 +4275,7 @@
         <v>35.314239999999998</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="67" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="6" t="s">
         <v>153</v>
       </c>
@@ -4298,7 +4298,7 @@
         <v>35.330410000000001</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="68" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="6" t="s">
         <v>5</v>
       </c>
@@ -4321,7 +4321,7 @@
         <v>35.330410000000001</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="69" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="6" t="s">
         <v>24</v>
       </c>
@@ -4344,7 +4344,7 @@
         <v>35.3108</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="70" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="6" t="s">
         <v>18</v>
       </c>
@@ -4367,7 +4367,7 @@
         <v>35.297379999999997</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="71" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="6" t="s">
         <v>18</v>
       </c>
@@ -4390,7 +4390,7 @@
         <v>35.312640000000002</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="72" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="6" t="s">
         <v>18</v>
       </c>
@@ -4413,7 +4413,7 @@
         <v>35.297379999999997</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="73" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="6" t="s">
         <v>21</v>
       </c>
@@ -4436,7 +4436,7 @@
         <v>35.292389999999997</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="74" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="6" t="s">
         <v>18</v>
       </c>
@@ -4459,7 +4459,7 @@
         <v>35.293190000000003</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="75" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="6" t="s">
         <v>18</v>
       </c>
@@ -4482,7 +4482,7 @@
         <v>35.293089999999999</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="76" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="6" t="s">
         <v>129</v>
       </c>
@@ -4505,7 +4505,7 @@
         <v>35.313580000000002</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="77" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="6" t="s">
         <v>29</v>
       </c>
@@ -4528,7 +4528,7 @@
         <v>35.304639999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="78" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="6" t="s">
         <v>21</v>
       </c>
@@ -4551,7 +4551,7 @@
         <v>35.310679999999998</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="79" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="6" t="s">
         <v>18</v>
       </c>
@@ -4574,7 +4574,7 @@
         <v>35.310679999999998</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="80" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="6" t="s">
         <v>18</v>
       </c>
@@ -4597,7 +4597,7 @@
         <v>35.292389999999997</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="81" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="6" t="s">
         <v>32</v>
       </c>
@@ -4620,7 +4620,7 @@
         <v>35.312579999999997</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="82" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="6" t="s">
         <v>100</v>
       </c>
@@ -4643,7 +4643,7 @@
         <v>35.299759999999999</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="83" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="6" t="s">
         <v>185</v>
       </c>
@@ -4666,7 +4666,7 @@
         <v>35.294280000000001</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="84" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="6" t="s">
         <v>9</v>
       </c>
@@ -4689,7 +4689,7 @@
         <v>35.305810000000001</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="85" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A85" s="6" t="s">
         <v>190</v>
       </c>
@@ -4712,7 +4712,7 @@
         <v>35.308540000000001</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="86" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A86" s="6" t="s">
         <v>193</v>
       </c>
@@ -4735,7 +4735,7 @@
         <v>35.282780000000002</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="87" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A87" s="6" t="s">
         <v>18</v>
       </c>
@@ -4758,7 +4758,7 @@
         <v>35.293089999999999</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="88" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A88" s="6" t="s">
         <v>129</v>
       </c>
@@ -4781,7 +4781,7 @@
         <v>35.300980000000003</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="89" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A89" s="6" t="s">
         <v>18</v>
       </c>
@@ -4804,7 +4804,7 @@
         <v>35.29524</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="90" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A90" s="6" t="s">
         <v>9</v>
       </c>
@@ -4827,7 +4827,7 @@
         <v>35.30827</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="91" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A91" s="6" t="s">
         <v>32</v>
       </c>
@@ -4850,7 +4850,7 @@
         <v>35.316409999999998</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="92" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A92" s="6" t="s">
         <v>21</v>
       </c>
@@ -4873,7 +4873,7 @@
         <v>35.296619999999997</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="93" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A93" s="6" t="s">
         <v>190</v>
       </c>
@@ -4896,7 +4896,7 @@
         <v>35.305759999999999</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="94" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A94" s="6" t="s">
         <v>5</v>
       </c>
@@ -4919,7 +4919,7 @@
         <v>35.313769999999998</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="95" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A95" s="6" t="s">
         <v>5</v>
       </c>
@@ -4942,7 +4942,7 @@
         <v>35.291730000000001</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="96" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A96" s="6" t="s">
         <v>32</v>
       </c>
@@ -4965,7 +4965,7 @@
         <v>35.317880000000002</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="97" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A97" s="6" t="s">
         <v>47</v>
       </c>
@@ -4988,7 +4988,7 @@
         <v>35.299759999999999</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="98" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A98" s="6" t="s">
         <v>24</v>
       </c>
@@ -5011,7 +5011,7 @@
         <v>35.292389999999997</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="99" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A99" s="6" t="s">
         <v>5</v>
       </c>
@@ -5034,7 +5034,7 @@
         <v>35.29571</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="100" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A100" s="6" t="s">
         <v>5</v>
       </c>
@@ -5057,7 +5057,7 @@
         <v>35.30827</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="101" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A101" s="6" t="s">
         <v>18</v>
       </c>
@@ -5080,7 +5080,7 @@
         <v>35.289299999999997</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="102" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A102" s="6" t="s">
         <v>32</v>
       </c>
@@ -5103,7 +5103,7 @@
         <v>35.323689999999999</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="103" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A103" s="6" t="s">
         <v>24</v>
       </c>
@@ -5126,7 +5126,7 @@
         <v>35.301909999999999</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="104" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A104" s="6" t="s">
         <v>32</v>
       </c>
@@ -5149,7 +5149,7 @@
         <v>35.304049999999997</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="105" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A105" s="6" t="s">
         <v>32</v>
       </c>
@@ -5172,7 +5172,7 @@
         <v>35.313949999999998</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="106" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A106" s="6" t="s">
         <v>24</v>
       </c>
@@ -5195,7 +5195,7 @@
         <v>35.325420000000001</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="107" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A107" s="6" t="s">
         <v>21</v>
       </c>
@@ -5218,7 +5218,7 @@
         <v>35.307650000000002</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="108" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A108" s="6" t="s">
         <v>5</v>
       </c>
@@ -5241,7 +5241,7 @@
         <v>35.29204</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="109" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A109" s="6" t="s">
         <v>47</v>
       </c>
@@ -5264,7 +5264,7 @@
         <v>35.301220000000001</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="110" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A110" s="6" t="s">
         <v>32</v>
       </c>
@@ -5287,7 +5287,7 @@
         <v>35.288539999999998</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="111" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A111" s="6" t="s">
         <v>9</v>
       </c>
@@ -5310,7 +5310,7 @@
         <v>35.316099999999999</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="112" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A112" s="6" t="s">
         <v>9</v>
       </c>
@@ -5333,7 +5333,7 @@
         <v>35.297179999999997</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="113" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A113" s="6" t="s">
         <v>5</v>
       </c>
@@ -5356,7 +5356,7 @@
         <v>35.300930000000001</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="114" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A114" s="6" t="s">
         <v>153</v>
       </c>
@@ -5379,7 +5379,7 @@
         <v>35.296219999999998</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="115" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A115" s="6" t="s">
         <v>5</v>
       </c>
@@ -5402,7 +5402,7 @@
         <v>35.303139999999999</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="116" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A116" s="6" t="s">
         <v>24</v>
       </c>
@@ -5425,7 +5425,7 @@
         <v>35.294339999999998</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="117" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A117" s="6" t="s">
         <v>9</v>
       </c>
@@ -5448,7 +5448,7 @@
         <v>35.30827</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="118" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A118" s="6" t="s">
         <v>5</v>
       </c>
@@ -5471,7 +5471,7 @@
         <v>35.291870000000003</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="119" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A119" s="6" t="s">
         <v>15</v>
       </c>
@@ -5494,7 +5494,7 @@
         <v>35.30827</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="120" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A120" s="6" t="s">
         <v>9</v>
       </c>
@@ -5517,7 +5517,7 @@
         <v>35.307810000000003</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="121" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A121" s="6" t="s">
         <v>38</v>
       </c>
@@ -5540,7 +5540,7 @@
         <v>35.307830000000003</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="122" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A122" s="6" t="s">
         <v>47</v>
       </c>
@@ -5563,7 +5563,7 @@
         <v>35.293089999999999</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="123" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A123" s="6" t="s">
         <v>47</v>
       </c>
@@ -5586,7 +5586,7 @@
         <v>35.301909999999999</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="124" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A124" s="6" t="s">
         <v>9</v>
       </c>
@@ -5609,7 +5609,7 @@
         <v>35.313749999999999</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="125" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A125" s="6" t="s">
         <v>32</v>
       </c>
@@ -5632,7 +5632,7 @@
         <v>35.30827</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="126" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A126" s="6" t="s">
         <v>47</v>
       </c>
@@ -5655,7 +5655,7 @@
         <v>35.300980000000003</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="127" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A127" s="6" t="s">
         <v>5</v>
       </c>
@@ -5678,7 +5678,7 @@
         <v>35.307220000000001</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="128" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A128" s="6" t="s">
         <v>5</v>
       </c>
@@ -5701,7 +5701,7 @@
         <v>35.314660000000003</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="129" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A129" s="6" t="s">
         <v>9</v>
       </c>
@@ -5724,7 +5724,7 @@
         <v>35.29851</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="130" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A130" s="6" t="s">
         <v>100</v>
       </c>
@@ -5747,7 +5747,7 @@
         <v>35.313749999999999</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="131" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A131" s="6" t="s">
         <v>21</v>
       </c>
@@ -5770,7 +5770,7 @@
         <v>35.30827</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="132" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A132" s="6" t="s">
         <v>21</v>
       </c>
@@ -5793,7 +5793,7 @@
         <v>35.298839999999998</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="133" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A133" s="6" t="s">
         <v>9</v>
       </c>
@@ -5816,7 +5816,7 @@
         <v>35.312730000000002</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="134" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A134" s="6" t="s">
         <v>24</v>
       </c>
@@ -5839,7 +5839,7 @@
         <v>35.330620000000003</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="135" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A135" s="6" t="s">
         <v>12</v>
       </c>
@@ -5862,7 +5862,7 @@
         <v>35.330379999999998</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="136" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A136" s="6" t="s">
         <v>47</v>
       </c>
@@ -5885,7 +5885,7 @@
         <v>35.298250000000003</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="137" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A137" s="6" t="s">
         <v>9</v>
       </c>
@@ -5908,7 +5908,7 @@
         <v>35.317489999999999</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="138" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A138" s="6" t="s">
         <v>12</v>
       </c>
@@ -5931,7 +5931,7 @@
         <v>35.302120000000002</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="139" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A139" s="6" t="s">
         <v>5</v>
       </c>
@@ -5954,7 +5954,7 @@
         <v>35.293089999999999</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="140" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A140" s="6" t="s">
         <v>9</v>
       </c>
@@ -5977,7 +5977,7 @@
         <v>35.298870000000001</v>
       </c>
     </row>
-    <row r="141" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="141" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A141" s="6" t="s">
         <v>47</v>
       </c>
@@ -6000,7 +6000,7 @@
         <v>35.289810000000003</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="142" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A142" s="6" t="s">
         <v>32</v>
       </c>
@@ -6023,7 +6023,7 @@
         <v>35.28633</v>
       </c>
     </row>
-    <row r="143" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="143" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A143" s="6" t="s">
         <v>73</v>
       </c>
@@ -6046,7 +6046,7 @@
         <v>35.296709999999997</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="144" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A144" s="6" t="s">
         <v>310</v>
       </c>
@@ -6069,7 +6069,7 @@
         <v>35.305480000000003</v>
       </c>
     </row>
-    <row r="145" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="145" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A145" s="6" t="s">
         <v>18</v>
       </c>
@@ -6092,7 +6092,7 @@
         <v>35.293089999999999</v>
       </c>
     </row>
-    <row r="146" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="146" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A146" s="6" t="s">
         <v>9</v>
       </c>
@@ -6115,7 +6115,7 @@
         <v>35.31561</v>
       </c>
     </row>
-    <row r="147" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="147" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A147" s="6" t="s">
         <v>47</v>
       </c>
@@ -6138,7 +6138,7 @@
         <v>35.304049999999997</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="148" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A148" s="6" t="s">
         <v>12</v>
       </c>
@@ -6161,7 +6161,7 @@
         <v>35.318350000000002</v>
       </c>
     </row>
-    <row r="149" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="149" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A149" s="6" t="s">
         <v>32</v>
       </c>
@@ -6184,7 +6184,7 @@
         <v>35.293030000000002</v>
       </c>
     </row>
-    <row r="150" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="150" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A150" s="6" t="s">
         <v>21</v>
       </c>
@@ -6207,7 +6207,7 @@
         <v>35.312640000000002</v>
       </c>
     </row>
-    <row r="151" spans="1:7" ht="20.100000000000001" customHeight="1">
+    <row r="151" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A151" s="6" t="s">
         <v>32</v>
       </c>

</xml_diff>